<commit_message>
Re doing data as there was an error
</commit_message>
<xml_diff>
--- a/Team-Data/2008-09/10-29-2008-09.xlsx
+++ b/Team-Data/2008-09/10-29-2008-09.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B1:BF1"/>
+  <dimension ref="A1:BF7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,6 +720,1098 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1610612738</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>48</v>
+      </c>
+      <c r="I2" t="n">
+        <v>33</v>
+      </c>
+      <c r="J2" t="n">
+        <v>74</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.446</v>
+      </c>
+      <c r="L2" t="n">
+        <v>3</v>
+      </c>
+      <c r="M2" t="n">
+        <v>14</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.214</v>
+      </c>
+      <c r="O2" t="n">
+        <v>21</v>
+      </c>
+      <c r="P2" t="n">
+        <v>34</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.618</v>
+      </c>
+      <c r="R2" t="n">
+        <v>10</v>
+      </c>
+      <c r="S2" t="n">
+        <v>26</v>
+      </c>
+      <c r="T2" t="n">
+        <v>36</v>
+      </c>
+      <c r="U2" t="n">
+        <v>16</v>
+      </c>
+      <c r="V2" t="n">
+        <v>17</v>
+      </c>
+      <c r="W2" t="n">
+        <v>10</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>28</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>26</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>90</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>6</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>5</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>4</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE2" t="inlineStr">
+        <is>
+          <t>Boston Celtics</t>
+        </is>
+      </c>
+      <c r="BF2" t="inlineStr">
+        <is>
+          <t>2008-10-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1610612741</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>48</v>
+      </c>
+      <c r="I3" t="n">
+        <v>35</v>
+      </c>
+      <c r="J3" t="n">
+        <v>69</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.507</v>
+      </c>
+      <c r="L3" t="n">
+        <v>5</v>
+      </c>
+      <c r="M3" t="n">
+        <v>12</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="O3" t="n">
+        <v>33</v>
+      </c>
+      <c r="P3" t="n">
+        <v>44</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R3" t="n">
+        <v>14</v>
+      </c>
+      <c r="S3" t="n">
+        <v>26</v>
+      </c>
+      <c r="T3" t="n">
+        <v>40</v>
+      </c>
+      <c r="U3" t="n">
+        <v>27</v>
+      </c>
+      <c r="V3" t="n">
+        <v>19</v>
+      </c>
+      <c r="W3" t="n">
+        <v>9</v>
+      </c>
+      <c r="X3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>108</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>3</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE3" t="inlineStr">
+        <is>
+          <t>Chicago Bulls</t>
+        </is>
+      </c>
+      <c r="BF3" t="inlineStr">
+        <is>
+          <t>2008-10-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1610612739</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="n">
+        <v>48</v>
+      </c>
+      <c r="I4" t="n">
+        <v>29</v>
+      </c>
+      <c r="J4" t="n">
+        <v>68</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.426</v>
+      </c>
+      <c r="L4" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" t="n">
+        <v>15</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="O4" t="n">
+        <v>24</v>
+      </c>
+      <c r="P4" t="n">
+        <v>33</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.727</v>
+      </c>
+      <c r="R4" t="n">
+        <v>8</v>
+      </c>
+      <c r="S4" t="n">
+        <v>33</v>
+      </c>
+      <c r="T4" t="n">
+        <v>41</v>
+      </c>
+      <c r="U4" t="n">
+        <v>16</v>
+      </c>
+      <c r="V4" t="n">
+        <v>22</v>
+      </c>
+      <c r="W4" t="n">
+        <v>8</v>
+      </c>
+      <c r="X4" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>28</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>85</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>-5</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>2</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>5</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE4" t="inlineStr">
+        <is>
+          <t>Cleveland Cavaliers</t>
+        </is>
+      </c>
+      <c r="BF4" t="inlineStr">
+        <is>
+          <t>2008-10-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1610612747</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>48</v>
+      </c>
+      <c r="I5" t="n">
+        <v>37</v>
+      </c>
+      <c r="J5" t="n">
+        <v>79</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.468</v>
+      </c>
+      <c r="L5" t="n">
+        <v>7</v>
+      </c>
+      <c r="M5" t="n">
+        <v>10</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="O5" t="n">
+        <v>15</v>
+      </c>
+      <c r="P5" t="n">
+        <v>18</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="R5" t="n">
+        <v>9</v>
+      </c>
+      <c r="S5" t="n">
+        <v>40</v>
+      </c>
+      <c r="T5" t="n">
+        <v>49</v>
+      </c>
+      <c r="U5" t="n">
+        <v>19</v>
+      </c>
+      <c r="V5" t="n">
+        <v>15</v>
+      </c>
+      <c r="W5" t="n">
+        <v>8</v>
+      </c>
+      <c r="X5" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>96</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>5</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE5" t="inlineStr">
+        <is>
+          <t>Los Angeles Lakers</t>
+        </is>
+      </c>
+      <c r="BF5" t="inlineStr">
+        <is>
+          <t>2008-10-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1610612749</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>48</v>
+      </c>
+      <c r="I6" t="n">
+        <v>37</v>
+      </c>
+      <c r="J6" t="n">
+        <v>78</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6</v>
+      </c>
+      <c r="M6" t="n">
+        <v>14</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.429</v>
+      </c>
+      <c r="O6" t="n">
+        <v>15</v>
+      </c>
+      <c r="P6" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R6" t="n">
+        <v>13</v>
+      </c>
+      <c r="S6" t="n">
+        <v>19</v>
+      </c>
+      <c r="T6" t="n">
+        <v>32</v>
+      </c>
+      <c r="U6" t="n">
+        <v>21</v>
+      </c>
+      <c r="V6" t="n">
+        <v>19</v>
+      </c>
+      <c r="W6" t="n">
+        <v>5</v>
+      </c>
+      <c r="X6" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>30</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>18</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>95</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>-13</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>2</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>6</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>5</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>6</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>4</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>3</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>5</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE6" t="inlineStr">
+        <is>
+          <t>Milwaukee Bucks</t>
+        </is>
+      </c>
+      <c r="BF6" t="inlineStr">
+        <is>
+          <t>2008-10-29</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1610612757</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>48</v>
+      </c>
+      <c r="I7" t="n">
+        <v>29</v>
+      </c>
+      <c r="J7" t="n">
+        <v>84</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="L7" t="n">
+        <v>10</v>
+      </c>
+      <c r="M7" t="n">
+        <v>24</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.417</v>
+      </c>
+      <c r="O7" t="n">
+        <v>8</v>
+      </c>
+      <c r="P7" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.571</v>
+      </c>
+      <c r="R7" t="n">
+        <v>13</v>
+      </c>
+      <c r="S7" t="n">
+        <v>31</v>
+      </c>
+      <c r="T7" t="n">
+        <v>44</v>
+      </c>
+      <c r="U7" t="n">
+        <v>19</v>
+      </c>
+      <c r="V7" t="n">
+        <v>14</v>
+      </c>
+      <c r="W7" t="n">
+        <v>8</v>
+      </c>
+      <c r="X7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>17</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>76</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>-20</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>5</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>6</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>6</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>10</v>
+      </c>
+      <c r="BE7" t="inlineStr">
+        <is>
+          <t>Portland Trail Blazers</t>
+        </is>
+      </c>
+      <c r="BF7" t="inlineStr">
+        <is>
+          <t>2008-10-29</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>